<commit_message>
[release]release sdk 4.8.8 for liteos
</commit_message>
<xml_diff>
--- a/docs/cn/IPC SDK内存占用统计与说明.xlsx
+++ b/docs/cn/IPC SDK内存占用统计与说明.xlsx
@@ -173,8 +173,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -192,8 +192,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -215,7 +216,53 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,11 +276,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -253,76 +321,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -363,13 +363,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,163 +477,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -566,11 +566,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -593,38 +623,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,8 +647,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -669,10 +669,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -681,137 +681,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -821,12 +821,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1171,8 +1165,8 @@
   <sheetPr/>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
@@ -1232,7 +1226,7 @@
       <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
@@ -1255,10 +1249,10 @@
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
@@ -1281,13 +1275,13 @@
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>1</v>
       </c>
       <c r="C9" s="2">
         <v>0.8</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -1298,17 +1292,17 @@
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="8">
         <v>10</v>
       </c>
       <c r="C10" s="2">
         <f>B2*B10/8/1024</f>
         <v>1.875</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="9" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1316,17 +1310,17 @@
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="8">
         <v>10</v>
       </c>
       <c r="C11" s="2">
         <f>B3*B11/8/1024</f>
         <v>0.625</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="9" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1334,17 +1328,17 @@
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="8">
         <v>10</v>
       </c>
       <c r="C12" s="2">
         <f>B4*B12/8/1024</f>
         <v>0.152587890625</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1352,17 +1346,17 @@
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="6">
         <v>10</v>
       </c>
       <c r="C13" s="2">
         <f>(B2+B4)*(B13+1)/8/1024+B6/1024+B5/1024</f>
         <v>2.6209716796875</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1370,17 +1364,17 @@
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="10">
         <v>6</v>
       </c>
       <c r="C14" s="2">
         <f>B2*B14/8/1024+B4*B14/8/1024</f>
         <v>1.216552734375</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1388,17 +1382,17 @@
       <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="8">
         <v>3</v>
       </c>
       <c r="C15" s="2">
         <f>0.8*B15</f>
         <v>2.4</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="9" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1406,17 +1400,17 @@
       <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="6">
         <v>1</v>
       </c>
       <c r="C16" s="2">
         <f>B5*2/1024</f>
         <v>0.1953125</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="9" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1424,17 +1418,17 @@
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="10">
         <v>1</v>
       </c>
       <c r="C17" s="2">
         <f>B5*2/1024*B17</f>
         <v>0.1953125</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="9" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1442,17 +1436,17 @@
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="6">
         <v>1</v>
       </c>
       <c r="C18" s="2">
-        <f>B6/1024*2*B18*B18</f>
+        <f>B6/1024*2*B18</f>
         <v>0.5859375</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1460,17 +1454,17 @@
       <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="8">
         <v>1</v>
       </c>
       <c r="C19" s="2">
         <f>B5*2/1024*B19</f>
         <v>0.1953125</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="9" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1478,7 +1472,7 @@
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="9"/>
+      <c r="D20" s="7"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
@@ -1488,11 +1482,11 @@
       <c r="B21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="11">
         <f>SUM(C9:C20)</f>
         <v>10.8619873046875</v>
       </c>
-      <c r="D21" s="14"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="2" t="s">
         <v>41</v>
       </c>
@@ -1507,17 +1501,17 @@
       </c>
     </row>
     <row r="24" spans="2:4">
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
     </row>
     <row r="28" spans="3:4">
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
     </row>
     <row r="29" spans="3:4">
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>